<commit_message>
Actrualizacion Codigo agreagando boxplot
</commit_message>
<xml_diff>
--- a/Datos/Diccionario de datos/Catalogo de variables/ESTADO_CONYUGAL.xlsx
+++ b/Datos/Diccionario de datos/Catalogo de variables/ESTADO_CONYUGAL.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\benja\Downloads\sinac_catalogos_2020\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\benja\OneDrive\Documentos\GitHub\ProyectoFinal_IC\Datos\Diccionario de datos\Catalogo de variables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F159CBF5-3ABC-4A26-A3A9-90C77CE168F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95B1EFCE-F0B3-458E-86CB-2CC05CC0A9AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9330" yWindow="2085" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
   <si>
     <t>NO ESPECIFICADO</t>
   </si>
@@ -58,6 +58,24 @@
   </si>
   <si>
     <t>SEPARADO(A)</t>
+  </si>
+  <si>
+    <t>CASADA</t>
+  </si>
+  <si>
+    <t>SOLTERA</t>
+  </si>
+  <si>
+    <t>DIVORCIADA</t>
+  </si>
+  <si>
+    <t>VIUDA</t>
+  </si>
+  <si>
+    <t>SEPARADA</t>
+  </si>
+  <si>
+    <t>UNIÓN LIBRE</t>
   </si>
 </sst>
 </file>
@@ -81,27 +99,15 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.14999847407452621"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.249977111117893"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="7">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -110,73 +116,16 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
+      <left style="thin">
         <color indexed="64"/>
       </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="medium">
+      <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="medium">
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -185,32 +134,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -491,10 +423,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A1:XFD3"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -503,83 +435,147 @@
     <col min="2" max="2" width="19.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="5">
+      <c r="A2" s="2">
         <v>0</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="4">
+      <c r="A3" s="2">
         <v>1</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="4">
+      <c r="A4" s="2">
         <v>2</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="4">
+      <c r="A5" s="2">
         <v>3</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="4">
+      <c r="A6" s="2">
         <v>4</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="4">
+      <c r="A7" s="2">
         <v>5</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="4">
+      <c r="A8" s="2">
         <v>6</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="2" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="5">
+      <c r="A9" s="2">
         <v>8</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="7">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
         <v>9</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="3">
+        <v>11</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="3">
+        <v>12</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="3">
+        <v>13</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="3">
+        <v>14</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="3">
+        <v>15</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="3">
+        <v>16</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="3">
+        <v>88</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="3">
+        <v>99</v>
+      </c>
+      <c r="B18" s="2" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>